<commit_message>
Fixed compiler problems, created player constructors, implemented failing player test
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="551" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="551"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="31">
   <si>
     <t>C</t>
   </si>
@@ -107,16 +106,16 @@
   </si>
   <si>
     <t>Dark Blue: Test Door Exits</t>
+  </si>
+  <si>
+    <t>Dark Purple: Player Starts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,23 +123,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,9 +197,21 @@
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -223,93 +219,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -368,29 +330,324 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AA36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="5.71255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="8.5748987854251"/>
+    <col min="1" max="35" width="5.7109375"/>
+    <col min="36" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +657,7 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -436,7 +693,7 @@
       <c r="O1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -469,11 +726,11 @@
       <c r="Z1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA1" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,11 +809,11 @@
       <c r="Z2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,11 +892,11 @@
       <c r="Z3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AA3" s="6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,14 +972,14 @@
       <c r="Y4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Z4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,11 +1058,11 @@
       <c r="Z5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AA5" s="6" t="n">
+      <c r="AA5" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -884,12 +1141,12 @@
       <c r="Z6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA6" s="6" t="n">
+      <c r="AA6" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -967,11 +1224,11 @@
       <c r="Z7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA7" s="6" t="n">
+      <c r="AA7" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1050,11 +1307,11 @@
       <c r="Z8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AA8" s="6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA8" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1133,11 +1390,11 @@
       <c r="Z9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA9" s="6" t="n">
+      <c r="AA9" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1216,11 +1473,11 @@
       <c r="Z10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA10" s="6" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA10" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1299,11 +1556,11 @@
       <c r="Z11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA11" s="6" t="n">
+      <c r="AA11" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1382,11 +1639,11 @@
       <c r="Z12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA12" s="6" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA12" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1465,11 +1722,11 @@
       <c r="Z13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AA13" s="6" t="n">
+      <c r="AA13" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1548,11 +1805,11 @@
       <c r="Z14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA14" s="6" t="n">
+      <c r="AA14" s="6">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1631,11 +1888,11 @@
       <c r="Z15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA15" s="6" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA15" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1714,11 +1971,11 @@
       <c r="Z16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA16" s="6" t="n">
+      <c r="AA16" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1797,11 +2054,11 @@
       <c r="Z17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA17" s="6" t="n">
+      <c r="AA17" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1880,11 +2137,11 @@
       <c r="Z18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA18" s="6" t="n">
+      <c r="AA18" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1963,11 +2220,11 @@
       <c r="Z19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA19" s="6" t="n">
+      <c r="AA19" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2046,11 +2303,11 @@
       <c r="Z20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA20" s="6" t="n">
+      <c r="AA20" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -2126,14 +2383,14 @@
       <c r="Y21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Z21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="6" t="n">
+      <c r="Z21" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2212,11 +2469,11 @@
       <c r="Z22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AA22" s="6" t="n">
+      <c r="AA22" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2295,11 +2552,11 @@
       <c r="Z23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA23" s="6" t="n">
+      <c r="AA23" s="6">
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2378,11 +2635,11 @@
       <c r="Z24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA24" s="6" t="n">
+      <c r="AA24" s="6">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -2461,11 +2718,11 @@
       <c r="Z25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA25" s="6" t="n">
+      <c r="AA25" s="6">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2747,7 @@
       <c r="H26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="13" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="10" t="s">
@@ -2544,190 +2801,170 @@
       <c r="Z26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA26" s="6" t="n">
+      <c r="AA26" s="6">
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B27" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D27" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E27" s="6" t="n">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>0</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6">
         <v>4</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="6">
         <v>5</v>
       </c>
-      <c r="G27" s="6" t="n">
+      <c r="G27" s="6">
         <v>6</v>
       </c>
-      <c r="H27" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="I27" s="6" t="n">
+      <c r="H27" s="6">
+        <v>7</v>
+      </c>
+      <c r="I27" s="6">
         <v>8</v>
       </c>
-      <c r="J27" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="K27" s="6" t="n">
+      <c r="J27" s="6">
+        <v>9</v>
+      </c>
+      <c r="K27" s="6">
         <v>10</v>
       </c>
-      <c r="L27" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="M27" s="6" t="n">
+      <c r="L27" s="6">
+        <v>11</v>
+      </c>
+      <c r="M27" s="6">
         <v>12</v>
       </c>
-      <c r="N27" s="6" t="n">
+      <c r="N27" s="6">
         <v>13</v>
       </c>
-      <c r="O27" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="P27" s="6" t="n">
+      <c r="O27" s="6">
+        <v>14</v>
+      </c>
+      <c r="P27" s="6">
         <v>15</v>
       </c>
-      <c r="Q27" s="6" t="n">
+      <c r="Q27" s="6">
         <v>16</v>
       </c>
-      <c r="R27" s="6" t="n">
+      <c r="R27" s="6">
         <v>17</v>
       </c>
-      <c r="S27" s="6" t="n">
+      <c r="S27" s="6">
         <v>18</v>
       </c>
-      <c r="T27" s="6" t="n">
+      <c r="T27" s="6">
         <v>19</v>
       </c>
-      <c r="U27" s="6" t="n">
+      <c r="U27" s="6">
         <v>20</v>
       </c>
-      <c r="V27" s="6" t="n">
+      <c r="V27" s="6">
         <v>21</v>
       </c>
-      <c r="W27" s="6" t="n">
+      <c r="W27" s="6">
         <v>22</v>
       </c>
-      <c r="X27" s="6" t="n">
+      <c r="X27" s="6">
         <v>23</v>
       </c>
-      <c r="Y27" s="6" t="n">
+      <c r="Y27" s="6">
         <v>24</v>
       </c>
-      <c r="Z27" s="6" t="n">
+      <c r="Z27" s="6">
         <v>25</v>
       </c>
       <c r="AA27" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>